<commit_message>
multivariate regression and correlation work
</commit_message>
<xml_diff>
--- a/Max SWE to spr Pre.xlsx
+++ b/Max SWE to spr Pre.xlsx
@@ -84,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -92,6 +92,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +410,8 @@
       <c r="A3" s="2">
         <v>-1461</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
         <v>0.958234784604712</v>
       </c>
     </row>
@@ -417,7 +419,8 @@
       <c r="A4" s="2">
         <v>-1095</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3">
         <v>1.28594412239378</v>
       </c>
     </row>
@@ -425,7 +428,8 @@
       <c r="A5" s="2">
         <v>-730</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>1.16773934183611</v>
       </c>
     </row>
@@ -433,7 +437,8 @@
       <c r="A6" s="2">
         <v>-365</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
         <v>0.930555326577276</v>
       </c>
     </row>
@@ -441,7 +446,8 @@
       <c r="A7" s="2">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
         <v>1.20774674501074</v>
       </c>
     </row>
@@ -449,7 +455,8 @@
       <c r="A8" s="2">
         <v>366</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>1.07630942992297</v>
       </c>
     </row>
@@ -457,7 +464,8 @@
       <c r="A9" s="2">
         <v>731</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>1.14964738049553</v>
       </c>
     </row>
@@ -465,7 +473,8 @@
       <c r="A10" s="2">
         <v>1096</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
         <v>1.44751669885749</v>
       </c>
     </row>
@@ -473,7 +482,8 @@
       <c r="A11" s="2">
         <v>1461</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
         <v>0.659992619149376</v>
       </c>
     </row>
@@ -481,7 +491,8 @@
       <c r="A12" s="2">
         <v>1827</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>1.6884549444693</v>
       </c>
     </row>
@@ -489,7 +500,8 @@
       <c r="A13" s="2">
         <v>2192</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>0.782194496932674</v>
       </c>
     </row>
@@ -497,7 +509,8 @@
       <c r="A14" s="2">
         <v>2557</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>0.977835886870144</v>
       </c>
     </row>
@@ -505,7 +518,8 @@
       <c r="A15" s="2">
         <v>2922</v>
       </c>
-      <c r="C15">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
         <v>1.08413281980199</v>
       </c>
     </row>
@@ -513,7 +527,8 @@
       <c r="A16" s="2">
         <v>3288</v>
       </c>
-      <c r="C16">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <v>0.86435829239966</v>
       </c>
     </row>
@@ -521,7 +536,8 @@
       <c r="A17" s="2">
         <v>3653</v>
       </c>
-      <c r="C17">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
         <v>0.864010997721067</v>
       </c>
     </row>
@@ -529,7 +545,8 @@
       <c r="A18" s="2">
         <v>4018</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3">
         <v>0.822429669497684</v>
       </c>
     </row>
@@ -537,7 +554,8 @@
       <c r="A19" s="2">
         <v>4383</v>
       </c>
-      <c r="C19">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
         <v>0.628445111692077</v>
       </c>
     </row>
@@ -545,7 +563,8 @@
       <c r="A20" s="2">
         <v>4749</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
         <v>0.832683925007164</v>
       </c>
     </row>
@@ -553,7 +572,8 @@
       <c r="A21" s="2">
         <v>5114</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
         <v>0.692927445731091</v>
       </c>
     </row>
@@ -561,7 +581,8 @@
       <c r="A22" s="2">
         <v>5479</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
         <v>0.759542793081277</v>
       </c>
     </row>
@@ -569,7 +590,8 @@
       <c r="A23" s="2">
         <v>5844</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
         <v>0.796312618337736</v>
       </c>
     </row>
@@ -577,7 +599,8 @@
       <c r="A24" s="2">
         <v>6210</v>
       </c>
-      <c r="C24">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
         <v>1.38416820223023</v>
       </c>
     </row>
@@ -585,7 +608,8 @@
       <c r="A25" s="2">
         <v>6575</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
         <v>1.11487710374212</v>
       </c>
     </row>
@@ -593,7 +617,8 @@
       <c r="A26" s="2">
         <v>6940</v>
       </c>
-      <c r="C26">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
         <v>0.845865772510009</v>
       </c>
     </row>
@@ -601,7 +626,8 @@
       <c r="A27" s="2">
         <v>7305</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
         <v>1.25084873441239</v>
       </c>
     </row>
@@ -609,7 +635,8 @@
       <c r="A28" s="2">
         <v>7671</v>
       </c>
-      <c r="C28">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
         <v>0.636426025269107</v>
       </c>
     </row>
@@ -617,7 +644,8 @@
       <c r="A29" s="2">
         <v>8036</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
         <v>0.98129804052366</v>
       </c>
     </row>
@@ -625,7 +653,8 @@
       <c r="A30" s="2">
         <v>8401</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
         <v>0.911741775166309</v>
       </c>
     </row>
@@ -633,7 +662,8 @@
       <c r="A31" s="2">
         <v>8766</v>
       </c>
-      <c r="C31">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
         <v>0.670864336306538</v>
       </c>
     </row>
@@ -641,7 +671,8 @@
       <c r="A32" s="2">
         <v>9132</v>
       </c>
-      <c r="C32">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
         <v>0.523172564970161</v>
       </c>
     </row>
@@ -649,7 +680,8 @@
       <c r="A33" s="2">
         <v>9497</v>
       </c>
-      <c r="C33">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3">
         <v>0.996815581457579</v>
       </c>
     </row>
@@ -657,7 +689,8 @@
       <c r="A34" s="2">
         <v>9862</v>
       </c>
-      <c r="C34">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3">
         <v>0.881872148956218</v>
       </c>
     </row>
@@ -665,7 +698,8 @@
       <c r="A35" s="2">
         <v>10227</v>
       </c>
-      <c r="C35">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
         <v>1.04564079606659</v>
       </c>
     </row>
@@ -673,7 +707,8 @@
       <c r="A36" s="2">
         <v>10593</v>
       </c>
-      <c r="C36">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3">
         <v>0.970266870292237</v>
       </c>
     </row>
@@ -681,7 +716,8 @@
       <c r="A37" s="2">
         <v>10958</v>
       </c>
-      <c r="C37">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3">
         <v>0.649180053441417</v>
       </c>
     </row>
@@ -689,7 +725,8 @@
       <c r="A38" s="2">
         <v>11323</v>
       </c>
-      <c r="C38">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3">
         <v>0.880327496712224</v>
       </c>
     </row>
@@ -697,7 +734,8 @@
       <c r="A39" s="2">
         <v>11688</v>
       </c>
-      <c r="C39">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3">
         <v>0.855506533067352</v>
       </c>
     </row>
@@ -705,7 +743,8 @@
       <c r="A40" s="2">
         <v>12054</v>
       </c>
-      <c r="C40">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3">
         <v>1.01514587805871</v>
       </c>
     </row>
@@ -713,7 +752,8 @@
       <c r="A41" s="2">
         <v>12419</v>
       </c>
-      <c r="C41">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3">
         <v>0.934430150389563</v>
       </c>
     </row>
@@ -721,7 +761,8 @@
       <c r="A42" s="2">
         <v>12784</v>
       </c>
-      <c r="C42">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3">
         <v>0.681077986609399</v>
       </c>
     </row>
@@ -729,7 +770,8 @@
       <c r="A43" s="2">
         <v>13149</v>
       </c>
-      <c r="C43">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3">
         <v>0.782144428789376</v>
       </c>
     </row>
@@ -737,7 +779,8 @@
       <c r="A44" s="2">
         <v>13515</v>
       </c>
-      <c r="C44">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3">
         <v>0.886354380866671</v>
       </c>
     </row>
@@ -745,7 +788,8 @@
       <c r="A45" s="2">
         <v>13880</v>
       </c>
-      <c r="C45">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3">
         <v>1.23991188633997</v>
       </c>
     </row>
@@ -753,7 +797,8 @@
       <c r="A46" s="2">
         <v>14245</v>
       </c>
-      <c r="C46">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3">
         <v>1.21304914099327</v>
       </c>
     </row>
@@ -761,7 +806,8 @@
       <c r="A47" s="2">
         <v>14610</v>
       </c>
-      <c r="C47">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3">
         <v>0.748065125669764</v>
       </c>
     </row>
@@ -769,7 +815,8 @@
       <c r="A48" s="2">
         <v>14976</v>
       </c>
-      <c r="C48">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3">
         <v>1.21643648283802</v>
       </c>
     </row>
@@ -777,7 +824,8 @@
       <c r="A49" s="2">
         <v>15341</v>
       </c>
-      <c r="C49">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3">
         <v>0.647227044857056</v>
       </c>
     </row>
@@ -785,7 +833,8 @@
       <c r="A50" s="2">
         <v>15706</v>
       </c>
-      <c r="C50">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3">
         <v>0.822731498097085</v>
       </c>
     </row>
@@ -793,7 +842,8 @@
       <c r="A51" s="2">
         <v>16071</v>
       </c>
-      <c r="C51">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3">
         <v>0.977356514107951</v>
       </c>
     </row>
@@ -801,7 +851,8 @@
       <c r="A52" s="2">
         <v>16437</v>
       </c>
-      <c r="C52">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3">
         <v>0.752068096590225</v>
       </c>
     </row>
@@ -809,7 +860,8 @@
       <c r="A53" s="2">
         <v>16802</v>
       </c>
-      <c r="C53">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3">
         <v>1.49927471305323</v>
       </c>
     </row>
@@ -817,7 +869,8 @@
       <c r="A54" s="2">
         <v>17167</v>
       </c>
-      <c r="C54">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3">
         <v>0.883718629799614</v>
       </c>
     </row>
@@ -825,7 +878,8 @@
       <c r="A55" s="2">
         <v>17532</v>
       </c>
-      <c r="C55">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3">
         <v>0.740616364436475</v>
       </c>
     </row>
@@ -833,7 +887,8 @@
       <c r="A56" s="2">
         <v>17898</v>
       </c>
-      <c r="C56">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3">
         <v>1.22009663195893</v>
       </c>
     </row>
@@ -841,7 +896,8 @@
       <c r="A57" s="2">
         <v>18263</v>
       </c>
-      <c r="C57">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3">
         <v>1.1515826344564</v>
       </c>
     </row>
@@ -849,7 +905,8 @@
       <c r="A58" s="2">
         <v>18628</v>
       </c>
-      <c r="C58">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3">
         <v>0.9722558434499</v>
       </c>
     </row>
@@ -857,7 +914,8 @@
       <c r="A59" s="2">
         <v>18993</v>
       </c>
-      <c r="C59">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3">
         <v>0.977235083911153</v>
       </c>
     </row>
@@ -865,7 +923,8 @@
       <c r="A60" s="2">
         <v>19359</v>
       </c>
-      <c r="C60">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3">
         <v>0.754747384350851</v>
       </c>
     </row>
@@ -873,7 +932,8 @@
       <c r="A61" s="2">
         <v>19724</v>
       </c>
-      <c r="C61">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3">
         <v>1.13920766188095</v>
       </c>
     </row>
@@ -881,7 +941,8 @@
       <c r="A62" s="2">
         <v>20089</v>
       </c>
-      <c r="C62">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3">
         <v>0.795052040069649</v>
       </c>
     </row>
@@ -889,7 +950,8 @@
       <c r="A63" s="2">
         <v>20454</v>
       </c>
-      <c r="C63">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3">
         <v>1.02161879047896</v>
       </c>
     </row>
@@ -897,7 +959,8 @@
       <c r="A64" s="2">
         <v>20820</v>
       </c>
-      <c r="C64">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3">
         <v>0.963648694121606</v>
       </c>
     </row>
@@ -905,7 +968,8 @@
       <c r="A65" s="2">
         <v>21185</v>
       </c>
-      <c r="C65">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3">
         <v>1.20717236061669</v>
       </c>
     </row>
@@ -913,7 +977,8 @@
       <c r="A66" s="2">
         <v>21550</v>
       </c>
-      <c r="C66">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3">
         <v>0.994383198038875</v>
       </c>
     </row>
@@ -921,7 +986,8 @@
       <c r="A67" s="2">
         <v>21915</v>
       </c>
-      <c r="C67">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3">
         <v>0.873562985160939</v>
       </c>
     </row>
@@ -929,7 +995,8 @@
       <c r="A68" s="2">
         <v>22281</v>
       </c>
-      <c r="C68">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3">
         <v>1.44179960683563</v>
       </c>
     </row>
@@ -937,7 +1004,8 @@
       <c r="A69" s="2">
         <v>22646</v>
       </c>
-      <c r="C69">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3">
         <v>1.53921880257811</v>
       </c>
     </row>
@@ -945,7 +1013,8 @@
       <c r="A70" s="2">
         <v>23011</v>
       </c>
-      <c r="C70">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3">
         <v>1.16110017010327</v>
       </c>
     </row>
@@ -953,7 +1022,8 @@
       <c r="A71" s="2">
         <v>23376</v>
       </c>
-      <c r="C71">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3">
         <v>1.26897620499996</v>
       </c>
     </row>
@@ -961,7 +1031,8 @@
       <c r="A72" s="2">
         <v>23742</v>
       </c>
-      <c r="C72">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3">
         <v>0.635423003635011</v>
       </c>
     </row>
@@ -969,7 +1040,8 @@
       <c r="A73" s="2">
         <v>24107</v>
       </c>
-      <c r="C73">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3">
         <v>0.534307639434033</v>
       </c>
     </row>
@@ -977,7 +1049,8 @@
       <c r="A74" s="2">
         <v>24472</v>
       </c>
-      <c r="C74">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3">
         <v>0.702870034887835</v>
       </c>
     </row>
@@ -985,7 +1058,8 @@
       <c r="A75" s="2">
         <v>24837</v>
       </c>
-      <c r="C75">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3">
         <v>0.721486811793027</v>
       </c>
     </row>
@@ -993,7 +1067,8 @@
       <c r="A76" s="2">
         <v>25203</v>
       </c>
-      <c r="C76">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3">
         <v>0.961844956485453</v>
       </c>
     </row>
@@ -1001,7 +1076,8 @@
       <c r="A77" s="2">
         <v>25568</v>
       </c>
-      <c r="C77">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3">
         <v>0.683481986032184</v>
       </c>
     </row>
@@ -1009,7 +1085,8 @@
       <c r="A78" s="2">
         <v>25933</v>
       </c>
-      <c r="C78">
+      <c r="B78" s="3"/>
+      <c r="C78" s="3">
         <v>0.802739792042631</v>
       </c>
     </row>
@@ -1017,7 +1094,8 @@
       <c r="A79" s="2">
         <v>26298</v>
       </c>
-      <c r="C79">
+      <c r="B79" s="3"/>
+      <c r="C79" s="3">
         <v>1.12312197299522</v>
       </c>
     </row>
@@ -1025,7 +1103,8 @@
       <c r="A80" s="2">
         <v>26664</v>
       </c>
-      <c r="C80">
+      <c r="B80" s="3"/>
+      <c r="C80" s="3">
         <v>1.30816065905162</v>
       </c>
     </row>
@@ -1033,7 +1112,8 @@
       <c r="A81" s="2">
         <v>27029</v>
       </c>
-      <c r="C81">
+      <c r="B81" s="3"/>
+      <c r="C81" s="3">
         <v>0.622528769218613</v>
       </c>
     </row>
@@ -1041,7 +1121,8 @@
       <c r="A82" s="2">
         <v>27394</v>
       </c>
-      <c r="C82">
+      <c r="B82" s="3"/>
+      <c r="C82" s="3">
         <v>1.27607805439763</v>
       </c>
     </row>
@@ -1049,7 +1130,8 @@
       <c r="A83" s="2">
         <v>27759</v>
       </c>
-      <c r="C83">
+      <c r="B83" s="3"/>
+      <c r="C83" s="3">
         <v>1.07239701367233</v>
       </c>
     </row>
@@ -1057,7 +1139,8 @@
       <c r="A84" s="2">
         <v>28125</v>
       </c>
-      <c r="C84">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3">
         <v>0.98192298603814</v>
       </c>
     </row>
@@ -1065,7 +1148,8 @@
       <c r="A85" s="2">
         <v>28490</v>
       </c>
-      <c r="C85">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3">
         <v>0.909462833866183</v>
       </c>
     </row>
@@ -1073,7 +1157,8 @@
       <c r="A86" s="2">
         <v>28855</v>
       </c>
-      <c r="C86">
+      <c r="B86" s="3"/>
+      <c r="C86" s="3">
         <v>0.827588848911552</v>
       </c>
     </row>
@@ -1081,7 +1166,8 @@
       <c r="A87" s="2">
         <v>29220</v>
       </c>
-      <c r="C87">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3">
         <v>1.28600904335174</v>
       </c>
     </row>
@@ -1089,7 +1175,8 @@
       <c r="A88" s="2">
         <v>29586</v>
       </c>
-      <c r="C88">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3">
         <v>0.878699742080151</v>
       </c>
     </row>
@@ -1097,10 +1184,10 @@
       <c r="A89" s="2">
         <v>29951</v>
       </c>
-      <c r="B89">
-        <v>0.219838518712738</v>
-      </c>
-      <c r="C89">
+      <c r="B89" s="3">
+        <v>0.319942707967653</v>
+      </c>
+      <c r="C89" s="3">
         <v>0.987281348641201</v>
       </c>
     </row>
@@ -1108,10 +1195,10 @@
       <c r="A90" s="2">
         <v>30316</v>
       </c>
-      <c r="B90">
-        <v>1.31759702305832</v>
-      </c>
-      <c r="C90">
+      <c r="B90" s="3">
+        <v>1.26080739784752</v>
+      </c>
+      <c r="C90" s="3">
         <v>1.1082080892601</v>
       </c>
     </row>
@@ -1119,10 +1206,10 @@
       <c r="A91" s="2">
         <v>30681</v>
       </c>
-      <c r="B91">
-        <v>0.881958542477644</v>
-      </c>
-      <c r="C91">
+      <c r="B91" s="3">
+        <v>0.85791746292027</v>
+      </c>
+      <c r="C91" s="3">
         <v>1.43001064009222</v>
       </c>
     </row>
@@ -1130,10 +1217,10 @@
       <c r="A92" s="2">
         <v>31047</v>
       </c>
-      <c r="B92">
-        <v>0.983456699291138</v>
-      </c>
-      <c r="C92">
+      <c r="B92" s="3">
+        <v>0.947301818860181</v>
+      </c>
+      <c r="C92" s="3">
         <v>1.38453653612197</v>
       </c>
     </row>
@@ -1141,10 +1228,10 @@
       <c r="A93" s="2">
         <v>31412</v>
       </c>
-      <c r="B93">
-        <v>1.35666002514005</v>
-      </c>
-      <c r="C93">
+      <c r="B93" s="3">
+        <v>1.28846965481699</v>
+      </c>
+      <c r="C93" s="3">
         <v>0.832585314136358</v>
       </c>
     </row>
@@ -1152,10 +1239,10 @@
       <c r="A94" s="2">
         <v>31777</v>
       </c>
-      <c r="B94">
-        <v>0.840497299842953</v>
-      </c>
-      <c r="C94">
+      <c r="B94" s="3">
+        <v>0.896294512233187</v>
+      </c>
+      <c r="C94" s="3">
         <v>1.2413677654665</v>
       </c>
     </row>
@@ -1163,10 +1250,10 @@
       <c r="A95" s="2">
         <v>32142</v>
       </c>
-      <c r="B95">
-        <v>0.760513131329529</v>
-      </c>
-      <c r="C95">
+      <c r="B95" s="3">
+        <v>0.735046197423501</v>
+      </c>
+      <c r="C95" s="3">
         <v>0.886612633429166</v>
       </c>
     </row>
@@ -1174,10 +1261,10 @@
       <c r="A96" s="2">
         <v>32508</v>
       </c>
-      <c r="B96">
-        <v>0.812387354203956</v>
-      </c>
-      <c r="C96">
+      <c r="B96" s="3">
+        <v>0.78654757081118</v>
+      </c>
+      <c r="C96" s="3">
         <v>1.02274772623291</v>
       </c>
     </row>
@@ -1185,10 +1272,10 @@
       <c r="A97" s="2">
         <v>32873</v>
       </c>
-      <c r="B97">
-        <v>1.36497968823006</v>
-      </c>
-      <c r="C97">
+      <c r="B97" s="3">
+        <v>1.28812170189913</v>
+      </c>
+      <c r="C97" s="3">
         <v>1.02937281598633</v>
       </c>
     </row>
@@ -1196,10 +1283,10 @@
       <c r="A98" s="2">
         <v>33238</v>
       </c>
-      <c r="B98">
-        <v>0.905539329581574</v>
-      </c>
-      <c r="C98">
+      <c r="B98" s="3">
+        <v>0.879004297625483</v>
+      </c>
+      <c r="C98" s="3">
         <v>1.12443180886415</v>
       </c>
     </row>
@@ -1207,10 +1294,10 @@
       <c r="A99" s="2">
         <v>33603</v>
       </c>
-      <c r="B99">
-        <v>0.591378639059433</v>
-      </c>
-      <c r="C99">
+      <c r="B99" s="3">
+        <v>0.660620239061344</v>
+      </c>
+      <c r="C99" s="3">
         <v>1.22664918258982</v>
       </c>
     </row>
@@ -1218,10 +1305,10 @@
       <c r="A100" s="2">
         <v>33969</v>
       </c>
-      <c r="B100">
-        <v>0.343226548698312</v>
-      </c>
-      <c r="C100">
+      <c r="B100" s="3">
+        <v>0.411072395397175</v>
+      </c>
+      <c r="C100" s="3">
         <v>0.76956394954223</v>
       </c>
     </row>
@@ -1229,10 +1316,10 @@
       <c r="A101" s="2">
         <v>34334</v>
       </c>
-      <c r="B101">
-        <v>1.20634439586806</v>
-      </c>
-      <c r="C101">
+      <c r="B101" s="3">
+        <v>1.06714674528137</v>
+      </c>
+      <c r="C101" s="3">
         <v>1.28023263629527</v>
       </c>
     </row>
@@ -1240,10 +1327,10 @@
       <c r="A102" s="2">
         <v>34699</v>
       </c>
-      <c r="B102">
-        <v>0.583937852562806</v>
-      </c>
-      <c r="C102">
+      <c r="B102" s="3">
+        <v>0.63404062328488</v>
+      </c>
+      <c r="C102" s="3">
         <v>0.876456988790492</v>
       </c>
     </row>
@@ -1251,10 +1338,10 @@
       <c r="A103" s="2">
         <v>35064</v>
       </c>
-      <c r="B103">
-        <v>0.866178129674202</v>
-      </c>
-      <c r="C103">
+      <c r="B103" s="3">
+        <v>0.939994807585226</v>
+      </c>
+      <c r="C103" s="3">
         <v>1.10453135920068</v>
       </c>
     </row>
@@ -1262,10 +1349,10 @@
       <c r="A104" s="2">
         <v>35430</v>
       </c>
-      <c r="B104">
-        <v>0.766210622802509</v>
-      </c>
-      <c r="C104">
+      <c r="B104" s="3">
+        <v>0.815625633851674</v>
+      </c>
+      <c r="C104" s="3">
         <v>1.57331861899758</v>
       </c>
     </row>
@@ -1273,10 +1360,10 @@
       <c r="A105" s="2">
         <v>35795</v>
       </c>
-      <c r="B105">
-        <v>1.14787711853592</v>
-      </c>
-      <c r="C105">
+      <c r="B105" s="3">
+        <v>1.1766592253762</v>
+      </c>
+      <c r="C105" s="3">
         <v>1.21635150096319</v>
       </c>
     </row>
@@ -1284,10 +1371,10 @@
       <c r="A106" s="2">
         <v>36160</v>
       </c>
-      <c r="B106">
-        <v>0.716663559178208</v>
-      </c>
-      <c r="C106">
+      <c r="B106" s="3">
+        <v>0.71692358859333</v>
+      </c>
+      <c r="C106" s="3">
         <v>1.18112632795072</v>
       </c>
     </row>
@@ -1295,10 +1382,10 @@
       <c r="A107" s="2">
         <v>36525</v>
       </c>
-      <c r="B107">
-        <v>1.68144940991303</v>
-      </c>
-      <c r="C107">
+      <c r="B107" s="3">
+        <v>1.58301179978123</v>
+      </c>
+      <c r="C107" s="3">
         <v>1.41289518304383</v>
       </c>
     </row>
@@ -1306,10 +1393,10 @@
       <c r="A108" s="2">
         <v>36891</v>
       </c>
-      <c r="B108">
-        <v>1.10249835579447</v>
-      </c>
-      <c r="C108">
+      <c r="B108" s="3">
+        <v>1.00422570244352</v>
+      </c>
+      <c r="C108" s="3">
         <v>1.00283439882211</v>
       </c>
     </row>
@@ -1317,10 +1404,10 @@
       <c r="A109" s="2">
         <v>37256</v>
       </c>
-      <c r="B109">
-        <v>0.543774877410827</v>
-      </c>
-      <c r="C109">
+      <c r="B109" s="3">
+        <v>0.584133663293382</v>
+      </c>
+      <c r="C109" s="3">
         <v>0.797924471763006</v>
       </c>
     </row>
@@ -1328,10 +1415,10 @@
       <c r="A110" s="2">
         <v>37621</v>
       </c>
-      <c r="B110">
-        <v>1.33381651066071</v>
-      </c>
-      <c r="C110">
+      <c r="B110" s="3">
+        <v>1.23819045818694</v>
+      </c>
+      <c r="C110" s="3">
         <v>0.921891070312114</v>
       </c>
     </row>
@@ -1339,10 +1426,10 @@
       <c r="A111" s="2">
         <v>37986</v>
       </c>
-      <c r="B111">
-        <v>0.517222557140751</v>
-      </c>
-      <c r="C111">
+      <c r="B111" s="3">
+        <v>0.700209581118728</v>
+      </c>
+      <c r="C111" s="3">
         <v>1.25036935957805</v>
       </c>
     </row>
@@ -1350,10 +1437,10 @@
       <c r="A112" s="2">
         <v>38352</v>
       </c>
-      <c r="B112">
-        <v>1.01415884029892</v>
-      </c>
-      <c r="C112">
+      <c r="B112" s="3">
+        <v>0.932687796310271</v>
+      </c>
+      <c r="C112" s="3">
         <v>0.823375180367925</v>
       </c>
     </row>
@@ -1361,10 +1448,10 @@
       <c r="A113" s="2">
         <v>38717</v>
       </c>
-      <c r="B113">
-        <v>0.365130747755574</v>
-      </c>
-      <c r="C113">
+      <c r="B113" s="3">
+        <v>0.485937419220427</v>
+      </c>
+      <c r="C113" s="3">
         <v>0.957222771065544</v>
       </c>
     </row>
@@ -1372,10 +1459,10 @@
       <c r="A114" s="2">
         <v>39082</v>
       </c>
-      <c r="B114">
-        <v>1.10188938171265</v>
-      </c>
-      <c r="C114">
+      <c r="B114" s="3">
+        <v>1.0271570135079</v>
+      </c>
+      <c r="C114" s="3">
         <v>0.856050526751741</v>
       </c>
     </row>
@@ -1383,10 +1470,10 @@
       <c r="A115" s="2">
         <v>39447</v>
       </c>
-      <c r="B115">
-        <v>0.811034056792866</v>
-      </c>
-      <c r="C115">
+      <c r="B115" s="3">
+        <v>0.87018627017785</v>
+      </c>
+      <c r="C115" s="3">
         <v>1.01053119628367</v>
       </c>
     </row>
@@ -1394,10 +1481,10 @@
       <c r="A116" s="2">
         <v>39813</v>
       </c>
-      <c r="B116">
-        <v>1.75735522677252</v>
-      </c>
-      <c r="C116">
+      <c r="B116" s="3">
+        <v>1.62770919992565</v>
+      </c>
+      <c r="C116" s="3">
         <v>0.9874835972026</v>
       </c>
     </row>
@@ -1405,10 +1492,10 @@
       <c r="A117" s="2">
         <v>40178</v>
       </c>
-      <c r="B117">
-        <v>1.15305265560657</v>
-      </c>
-      <c r="C117">
+      <c r="B117" s="3">
+        <v>1.08787479767359</v>
+      </c>
+      <c r="C117" s="3">
         <v>1.00196442227089</v>
       </c>
     </row>
@@ -1416,10 +1503,10 @@
       <c r="A118" s="2">
         <v>40543</v>
       </c>
-      <c r="B118">
-        <v>0.579676734690523</v>
-      </c>
-      <c r="C118">
+      <c r="B118" s="3">
+        <v>0.663064065015626</v>
+      </c>
+      <c r="C118" s="3">
         <v>1.12068958957651</v>
       </c>
     </row>
@@ -1427,10 +1514,10 @@
       <c r="A119" s="2">
         <v>40908</v>
       </c>
-      <c r="B119">
-        <v>1.14604447215659</v>
-      </c>
-      <c r="C119">
+      <c r="B119" s="3">
+        <v>1.20704867203892</v>
+      </c>
+      <c r="C119" s="3">
         <v>1.39897555822439</v>
       </c>
     </row>
@@ -1438,10 +1525,10 @@
       <c r="A120" s="2">
         <v>41274</v>
       </c>
-      <c r="B120">
-        <v>1.16106000843186</v>
-      </c>
-      <c r="C120">
+      <c r="B120" s="3">
+        <v>1.0714393869942</v>
+      </c>
+      <c r="C120" s="3">
         <v>1.41841948593172</v>
       </c>
     </row>
@@ -1449,10 +1536,10 @@
       <c r="A121" s="2">
         <v>41639</v>
       </c>
-      <c r="B121">
-        <v>0.94455510574753</v>
-      </c>
-      <c r="C121">
+      <c r="B121" s="3">
+        <v>0.892325260620877</v>
+      </c>
+      <c r="C121" s="3">
         <v>0.77049739577719</v>
       </c>
     </row>
@@ -1460,10 +1547,10 @@
       <c r="A122" s="2">
         <v>42004</v>
       </c>
-      <c r="B122">
-        <v>0.540967513715515</v>
-      </c>
-      <c r="C122">
+      <c r="B122" s="3">
+        <v>0.62910116215569</v>
+      </c>
+      <c r="C122" s="3">
         <v>1.58836412703687</v>
       </c>
     </row>
@@ -1471,7 +1558,8 @@
       <c r="A123" s="2">
         <v>42369</v>
       </c>
-      <c r="C123">
+      <c r="B123" s="3"/>
+      <c r="C123" s="3">
         <v>0.27984837551536</v>
       </c>
     </row>

</xml_diff>